<commit_message>
update time sheet in google docs instead: https://docs.google.com/spreadsheets/d/1jzOy9n22uh7I2h4f0l-50SltHpcKUZw7A2Mk0YPp40Y/edit#gid=1942548133
</commit_message>
<xml_diff>
--- a/Time Sheet/Project Time Sheet.xlsx
+++ b/Time Sheet/Project Time Sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hardik\Documents\GitHub\Weltec-Project\Time Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Local\patrick.cura2\Weltec-Project\Time Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25608" windowHeight="14472" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14475" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Kwinno Pinede" sheetId="4" r:id="rId4"/>
     <sheet name="Patrick Cura" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>Week</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -246,6 +246,12 @@
   </si>
   <si>
     <t>Update project proposal document</t>
+  </si>
+  <si>
+    <t>Tried making the code work in other machines. Encountered some compatibility issues and had to research how to go around it.</t>
+  </si>
+  <si>
+    <t>Helped edit the proposal. Formatted UI of sample code.</t>
   </si>
 </sst>
 </file>
@@ -738,15 +744,15 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="23.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.8984375" style="1"/>
-    <col min="2" max="2" width="22.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="16.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.8984375" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="22.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:7" ht="23.1" customHeight="1">
@@ -905,11 +911,11 @@
       </c>
       <c r="F8" s="3">
         <f>VLOOKUP(A8,'Patrick Cura'!A5:F103,6,0)</f>
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="23.1" customHeight="1">
@@ -1181,11 +1187,11 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G18" s="3">
         <f t="shared" si="1"/>
-        <v>159</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1209,15 +1215,15 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="23.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.8984375" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
     <col min="2" max="2" width="35" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.59765625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="75.625" style="2" customWidth="1"/>
     <col min="4" max="4" width="13" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.8984375" style="2"/>
+    <col min="5" max="5" width="10.875" style="2"/>
     <col min="6" max="6" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.8984375" style="2"/>
+    <col min="7" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="5" customFormat="1" ht="23.1" customHeight="1">
@@ -2464,11 +2470,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="F58:F64"/>
-    <mergeCell ref="F65:F71"/>
-    <mergeCell ref="F72:F78"/>
-    <mergeCell ref="F79:F85"/>
-    <mergeCell ref="F86:F92"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A43"/>
     <mergeCell ref="F93:F99"/>
     <mergeCell ref="A86:A92"/>
     <mergeCell ref="A93:A99"/>
@@ -2485,13 +2493,11 @@
     <mergeCell ref="A58:A64"/>
     <mergeCell ref="A65:A71"/>
     <mergeCell ref="A72:A78"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="F58:F64"/>
+    <mergeCell ref="F65:F71"/>
+    <mergeCell ref="F72:F78"/>
+    <mergeCell ref="F79:F85"/>
+    <mergeCell ref="F86:F92"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2508,13 +2514,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="23.1" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="31.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="105.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
@@ -3623,6 +3629,24 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="F2:F8"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="F9:F15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="F16:F22"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="F23:F29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="F30:F36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="F37:F43"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="F44:F50"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="F51:F57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="F58:F64"/>
     <mergeCell ref="A86:A92"/>
     <mergeCell ref="F86:F92"/>
     <mergeCell ref="A93:A99"/>
@@ -3633,24 +3657,6 @@
     <mergeCell ref="F72:F78"/>
     <mergeCell ref="A79:A85"/>
     <mergeCell ref="F79:F85"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="F44:F50"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="F51:F57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="F58:F64"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="F23:F29"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="F30:F36"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="F37:F43"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="F2:F8"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="F9:F15"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="F16:F22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3671,14 +3677,14 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="23.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.8984375" style="10"/>
-    <col min="2" max="2" width="31.8984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.59765625" style="10" customWidth="1"/>
-    <col min="4" max="5" width="10.8984375" style="10"/>
+    <col min="1" max="1" width="10.875" style="10"/>
+    <col min="2" max="2" width="31.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.625" style="10" customWidth="1"/>
+    <col min="4" max="5" width="10.875" style="10"/>
     <col min="6" max="6" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.8984375" style="10"/>
+    <col min="7" max="16384" width="10.875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.1" customHeight="1">
@@ -4753,6 +4759,24 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="F2:F8"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="F9:F15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="F16:F22"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="F23:F29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="F30:F36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="F37:F43"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="F44:F50"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="F51:F57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="F58:F64"/>
     <mergeCell ref="A86:A92"/>
     <mergeCell ref="F86:F92"/>
     <mergeCell ref="A93:A99"/>
@@ -4763,24 +4787,6 @@
     <mergeCell ref="F72:F78"/>
     <mergeCell ref="A79:A85"/>
     <mergeCell ref="F79:F85"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="F44:F50"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="F51:F57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="F58:F64"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="F23:F29"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="F30:F36"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="F37:F43"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="F2:F8"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="F9:F15"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="F16:F22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4796,20 +4802,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="23.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="27.19921875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="75.59765625" style="10" customWidth="1"/>
-    <col min="4" max="5" width="10.8984375" style="10"/>
+    <col min="1" max="1" width="3.375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="27.25" style="10" customWidth="1"/>
+    <col min="3" max="3" width="75.625" style="10" customWidth="1"/>
+    <col min="4" max="5" width="10.875" style="10"/>
     <col min="6" max="6" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.8984375" style="10"/>
+    <col min="7" max="16384" width="10.875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.1" customHeight="1">
@@ -5220,7 +5226,7 @@
       </c>
       <c r="F30" s="11">
         <f t="shared" ref="F30" si="0">SUM(E30:E36)</f>
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="23.1" customHeight="1">
@@ -5276,9 +5282,13 @@
       <c r="B35" s="6">
         <v>42595</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="E35" s="4">
+        <v>7</v>
+      </c>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:6" ht="23.1" customHeight="1">
@@ -5286,9 +5296,13 @@
       <c r="B36" s="6">
         <v>42596</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="E36" s="4">
+        <v>5</v>
+      </c>
       <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" ht="23.1" customHeight="1">
@@ -5968,6 +5982,24 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="F2:F8"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="F9:F15"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="F16:F22"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="F23:F29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="F30:F36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="F37:F43"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="F44:F50"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="F51:F57"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="F58:F64"/>
     <mergeCell ref="A86:A92"/>
     <mergeCell ref="F86:F92"/>
     <mergeCell ref="A93:A99"/>
@@ -5978,24 +6010,6 @@
     <mergeCell ref="F72:F78"/>
     <mergeCell ref="A79:A85"/>
     <mergeCell ref="F79:F85"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="F44:F50"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="F51:F57"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="F58:F64"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="F23:F29"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="F30:F36"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="F37:F43"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="F2:F8"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="F9:F15"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="F16:F22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>